<commit_message>
Updated schematics with I2C addresses
</commit_message>
<xml_diff>
--- a/Orcad/6089-103-RevB_summary_BOM_with_inventory.xlsx
+++ b/Orcad/6089-103-RevB_summary_BOM_with_inventory.xlsx
@@ -12059,8 +12059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12825,25 +12825,25 @@
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
       </c>
       <c r="O21" s="7">
         <f>M21-N21</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P21" s="10">
-        <v>0.86860000000000004</v>
+        <v>1.0406</v>
       </c>
       <c r="Q21" s="10">
         <f t="shared" si="7"/>
-        <v>6.9488000000000003</v>
+        <v>8.3247999999999998</v>
       </c>
       <c r="R21" s="3">
         <f t="shared" ref="R21" si="9">M21*P21</f>
-        <v>0</v>
+        <v>104.06</v>
       </c>
     </row>
     <row r="22" spans="2:29" ht="30" x14ac:dyDescent="0.25">
@@ -13311,11 +13311,11 @@
         <v>12</v>
       </c>
       <c r="N34" s="9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="O34" s="7">
         <f t="shared" ref="O34" si="18">M34-N34</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P34" s="10">
         <v>32.479999999999997</v>
@@ -13367,25 +13367,25 @@
       </c>
       <c r="L36" s="1"/>
       <c r="M36" s="9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N36" s="9">
         <v>0</v>
       </c>
       <c r="O36" s="7">
         <f t="shared" ref="O36" si="22">M36-N36</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P36" s="10">
-        <v>0.48480000000000001</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="Q36" s="10">
         <f>B36*P36</f>
-        <v>3.3936000000000002</v>
+        <v>2.9889999999999999</v>
       </c>
       <c r="R36" s="3">
         <f t="shared" ref="R36" si="23">M36*P36</f>
-        <v>0</v>
+        <v>42.699999999999996</v>
       </c>
     </row>
     <row r="38" spans="2:29" x14ac:dyDescent="0.25">
@@ -13480,7 +13480,7 @@
     <row r="43" spans="2:29" x14ac:dyDescent="0.25">
       <c r="Q43" s="10">
         <f>SUM(Q6:Q42)</f>
-        <v>931.42939999999987</v>
+        <v>932.40079999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>